<commit_message>
Se crea transacción de actualización de perfil
</commit_message>
<xml_diff>
--- a/Wappi/src/test/resources/datadriven/DataDriven.xlsx
+++ b/Wappi/src/test/resources/datadriven/DataDriven.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pruebas\Wolox\Prueba\Wappi\src\test\resources\datadriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2024C80E-6921-4866-B09C-A3E8950BFB63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBD782C-B0B2-4DD0-BDDC-18DA72AB2580}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OrderWithCoupon" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>firstName</t>
   </si>
@@ -77,9 +77,6 @@
     <t>bornDate</t>
   </si>
   <si>
-    <t>Gender</t>
-  </si>
-  <si>
     <t>gender</t>
   </si>
   <si>
@@ -99,13 +96,19 @@
   </si>
   <si>
     <t>Registrado exitosamente</t>
+  </si>
+  <si>
+    <t>06/11/1993</t>
+  </si>
+  <si>
+    <t>‪C:\Users\jorma\Desktop\img.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +126,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -151,16 +162,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -443,7 +457,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,66 +506,82 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47528F01-1761-4AD7-A2EE-37DA5B408CFC}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="9.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3">
-        <v>34279</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -564,13 +594,13 @@
           <x14:formula1>
             <xm:f>'Profile List'!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F2</xm:sqref>
+          <xm:sqref>H2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A850A98C-33A1-4EB4-880D-05E75ED4DC17}">
           <x14:formula1>
             <xm:f>'Profile List'!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E2</xm:sqref>
+          <xm:sqref>G2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -596,28 +626,28 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tarea para subir archivos a input type file
</commit_message>
<xml_diff>
--- a/Wappi/src/test/resources/datadriven/DataDriven.xlsx
+++ b/Wappi/src/test/resources/datadriven/DataDriven.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pruebas\Wolox\Prueba\Wappi\src\test\resources\datadriven\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Wappi\Wappi\src\test\resources\datadriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBD782C-B0B2-4DD0-BDDC-18DA72AB2580}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="OrderWithCoupon" sheetId="1" r:id="rId1"/>
     <sheet name="Profile" sheetId="4" r:id="rId2"/>
     <sheet name="Profile List" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -101,13 +100,13 @@
     <t>06/11/1993</t>
   </si>
   <si>
-    <t>‪C:\Users\jorma\Desktop\img.jpg</t>
+    <t>C:/Wappi/Wappi/img.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -452,7 +451,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -460,16 +459,16 @@
       <selection pane="bottomLeft" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -483,7 +482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -505,28 +504,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47528F01-1761-4AD7-A2EE-37DA5B408CFC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -555,7 +554,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -590,13 +589,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CA150BDE-F4DE-405C-957B-8E429DF09B79}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Profile List'!$B$2:$B$3</xm:f>
           </x14:formula1>
           <xm:sqref>H2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A850A98C-33A1-4EB4-880D-05E75ED4DC17}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Profile List'!$A$2:$A$4</xm:f>
           </x14:formula1>
@@ -609,19 +608,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F0BACC-8F2D-40B3-8598-59F1C189136C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -629,7 +628,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -637,7 +636,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -645,7 +644,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Se termina flujo de la transacción Pedir una orden con el cupón de bienvenida
</commit_message>
<xml_diff>
--- a/Wappi/src/test/resources/datadriven/DataDriven.xlsx
+++ b/Wappi/src/test/resources/datadriven/DataDriven.xlsx
@@ -1,38 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Wappi\Wappi\src\test\resources\datadriven\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pruebas\Wolox\Prueba\Wappi\src\test\resources\datadriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05EEC06-4904-4260-BE35-131CA7512F67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="528" yWindow="2604" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OrderWithCoupon" sheetId="1" r:id="rId1"/>
     <sheet name="Profile" sheetId="4" r:id="rId2"/>
-    <sheet name="Profile List" sheetId="5" r:id="rId3"/>
+    <sheet name="List" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>firstName</t>
   </si>
@@ -55,9 +50,6 @@
     <t>expectedResult</t>
   </si>
   <si>
-    <t>user</t>
-  </si>
-  <si>
     <t>Administrador</t>
   </si>
   <si>
@@ -67,9 +59,6 @@
     <t>Pan tajado</t>
   </si>
   <si>
-    <t>El cupón ha sido utilizado con éxito</t>
-  </si>
-  <si>
     <t>image</t>
   </si>
   <si>
@@ -101,12 +90,24 @@
   </si>
   <si>
     <t>C:/Wappi/Wappi/img.jpg</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>Aceite de Girasol</t>
+  </si>
+  <si>
+    <t>Jamón Premium</t>
+  </si>
+  <si>
+    <t>ha sido utilizado con éxito</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -451,89 +452,101 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B2"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{953A99F8-41B6-4948-BF8C-DE478949A0A5}">
+          <x14:formula1>
+            <xm:f>List!$D$2:$D$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -542,27 +555,27 @@
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -571,16 +584,16 @@
         <v>5</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -589,15 +602,15 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
-            <xm:f>'Profile List'!$B$2:$B$3</xm:f>
+            <xm:f>List!$B$2:$B$3</xm:f>
           </x14:formula1>
           <xm:sqref>H2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
-            <xm:f>'Profile List'!$A$2:$A$4</xm:f>
+            <xm:f>List!$A$2:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>G2</xm:sqref>
         </x14:dataValidation>
@@ -608,48 +621,62 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>19</v>
+      <c r="D4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se termina flujo de transacción de ordenamiento por criterios
</commit_message>
<xml_diff>
--- a/Wappi/src/test/resources/datadriven/DataDriven.xlsx
+++ b/Wappi/src/test/resources/datadriven/DataDriven.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pruebas\Wolox\Prueba\Wappi\src\test\resources\datadriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05EEC06-4904-4260-BE35-131CA7512F67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C98B20-E0C9-4BA2-8AE8-732F52D9CE45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="528" yWindow="2604" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OrderWithCoupon" sheetId="1" r:id="rId1"/>
     <sheet name="Profile" sheetId="4" r:id="rId2"/>
-    <sheet name="List" sheetId="5" r:id="rId3"/>
+    <sheet name="SortOffersByCirteria" sheetId="6" r:id="rId3"/>
+    <sheet name="List" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="38">
   <si>
     <t>firstName</t>
   </si>
@@ -83,9 +84,6 @@
     <t>Estados Unidos</t>
   </si>
   <si>
-    <t>Registrado exitosamente</t>
-  </si>
-  <si>
     <t>06/11/1993</t>
   </si>
   <si>
@@ -102,6 +100,48 @@
   </si>
   <si>
     <t>ha sido utilizado con éxito</t>
+  </si>
+  <si>
+    <t>criteria</t>
+  </si>
+  <si>
+    <t>clickQuantity</t>
+  </si>
+  <si>
+    <t>sortExpected</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Precio</t>
+  </si>
+  <si>
+    <t>Comercio</t>
+  </si>
+  <si>
+    <t>ASC</t>
+  </si>
+  <si>
+    <t>DESC</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
 </sst>
 </file>
@@ -457,21 +497,20 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -494,7 +533,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -518,11 +557,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -534,13 +573,12 @@
     <col min="6" max="6" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -563,11 +601,8 @@
       <c r="H1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -575,7 +610,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -584,16 +619,13 @@
         <v>5</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -621,11 +653,172 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F74C67CE-1D87-4DA3-91BE-7B8BF3266240}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9DFAD74D-BB35-420B-9E92-5F64074A2F8E}">
+          <x14:formula1>
+            <xm:f>List!$F$2:$F$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FA2FD685-78A8-4B37-90E3-F71AB38BF641}">
+          <x14:formula1>
+            <xm:f>List!$G$2:$G$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E7</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -634,7 +827,7 @@
     <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -644,8 +837,14 @@
       <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -653,10 +852,16 @@
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -666,13 +871,22 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se hacen ajustes de la transacción de actualización de perfil
</commit_message>
<xml_diff>
--- a/Wappi/src/test/resources/datadriven/DataDriven.xlsx
+++ b/Wappi/src/test/resources/datadriven/DataDriven.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pruebas\Wolox\Prueba\Wappi\src\test\resources\datadriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C98B20-E0C9-4BA2-8AE8-732F52D9CE45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA662D78-A543-43AB-85E9-FB9489A3E368}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OrderWithCoupon" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>06/11/1993</t>
   </si>
   <si>
-    <t>C:/Wappi/Wappi/img.jpg</t>
-  </si>
-  <si>
     <t>userName</t>
   </si>
   <si>
@@ -142,13 +139,16 @@
   </si>
   <si>
     <t>6</t>
+  </si>
+  <si>
+    <t>img.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,14 +166,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -202,19 +194,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -495,7 +484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
@@ -510,7 +499,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -533,7 +522,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -559,15 +548,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
@@ -578,7 +567,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -609,8 +598,8 @@
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>19</v>
+      <c r="C2" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -618,7 +607,7 @@
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -672,19 +661,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -695,13 +684,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -712,13 +701,13 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -729,13 +718,13 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -746,13 +735,13 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -763,13 +752,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -780,13 +769,13 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -838,10 +827,10 @@
         <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -852,13 +841,13 @@
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -872,10 +861,10 @@
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -883,10 +872,10 @@
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>